<commit_message>
updated docu for tmhm 24
</commit_message>
<xml_diff>
--- a/Patch/Crib Crystal Documentation.xlsx
+++ b/Patch/Crib Crystal Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwg11\cribxtal\Patch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7658A224-259D-48FE-8922-4B713AEDB2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72876883-3A11-441C-8AFA-485F54711051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="1171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="1172">
   <si>
     <t>Old Rod</t>
   </si>
@@ -3597,6 +3597,9 @@
   </si>
   <si>
     <t>Coin case is in Goldenrod Dept Store B1F (replaces Ether). Purchase coins in Game Corner. 4000 Coins each. Does not disappear after tutoring.</t>
+  </si>
+  <si>
+    <t>Clair (visit Blackthorn Gym after Dragon's Den)</t>
   </si>
 </sst>
 </file>
@@ -4957,6 +4960,18 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4993,29 +5008,17 @@
     <xf numFmtId="0" fontId="24" fillId="41" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5024,167 +5027,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="41">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5441,6 +5283,167 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5583,30 +5586,30 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BEE697BB-2F24-4E74-8F3D-2A9FBAE6D691}" name="Table1" displayName="Table1" ref="A1:B54" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BEE697BB-2F24-4E74-8F3D-2A9FBAE6D691}" name="Table1" displayName="Table1" ref="A1:B54" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:B54" xr:uid="{BEE697BB-2F24-4E74-8F3D-2A9FBAE6D691}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8C9A6D20-999F-4C20-8BA9-A3D392D7AA2C}" name="Move" dataDxfId="31" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{9270017D-0837-4E0E-B8F0-D1FA60219642}" name="Changes" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{8C9A6D20-999F-4C20-8BA9-A3D392D7AA2C}" name="Move" dataDxfId="8" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{9270017D-0837-4E0E-B8F0-D1FA60219642}" name="Changes" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{112E367D-7322-4ADF-82EE-F5FA265974CA}" name="Table7" displayName="Table7" ref="A1:C59" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{112E367D-7322-4ADF-82EE-F5FA265974CA}" name="Table7" displayName="Table7" ref="A1:C59" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5">
   <autoFilter ref="A1:C59" xr:uid="{112E367D-7322-4ADF-82EE-F5FA265974CA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{57E5FF2E-FB3F-4FA6-B52F-986ECCD16298}" name="Number" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{302A2C5F-E82E-4FAB-94DC-E2F79807C30A}" name="Name" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{1B872A69-F714-47C8-AEF0-0326E2707C4E}" name="Location (bold if changed)" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{57E5FF2E-FB3F-4FA6-B52F-986ECCD16298}" name="Number" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{302A2C5F-E82E-4FAB-94DC-E2F79807C30A}" name="Name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{1B872A69-F714-47C8-AEF0-0326E2707C4E}" name="Location (bold if changed)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5616,8 +5619,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4DE61D18-F3DB-48A2-942E-004065F17F28}" name="Table3" displayName="Table3" ref="A2:C32" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{3F2CCF71-D3CA-460E-8C1A-9BC91C192F05}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{4BB25EDA-360F-4595-BEE1-36E13E37F812}" name="Location" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{8C1B3EBC-0DA6-4AAB-B797-97FDB6258CD2}" name="Column1" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{4BB25EDA-360F-4595-BEE1-36E13E37F812}" name="Location" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{8C1B3EBC-0DA6-4AAB-B797-97FDB6258CD2}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7154,11 +7157,11 @@
       <c r="C32" s="1">
         <v>9</v>
       </c>
-      <c r="D32" s="208" t="s">
+      <c r="D32" s="212" t="s">
         <v>1127</v>
       </c>
-      <c r="E32" s="209"/>
-      <c r="F32" s="210"/>
+      <c r="E32" s="213"/>
+      <c r="F32" s="214"/>
     </row>
     <row r="33" spans="1:6" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -7170,9 +7173,9 @@
       <c r="C33" s="1">
         <v>9</v>
       </c>
-      <c r="D33" s="211"/>
-      <c r="E33" s="212"/>
-      <c r="F33" s="213"/>
+      <c r="D33" s="215"/>
+      <c r="E33" s="216"/>
+      <c r="F33" s="217"/>
     </row>
     <row r="34" spans="1:6" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -7184,9 +7187,9 @@
       <c r="C34">
         <v>13</v>
       </c>
-      <c r="D34" s="211"/>
-      <c r="E34" s="212"/>
-      <c r="F34" s="213"/>
+      <c r="D34" s="215"/>
+      <c r="E34" s="216"/>
+      <c r="F34" s="217"/>
     </row>
     <row r="35" spans="1:6" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -7198,9 +7201,9 @@
       <c r="C35">
         <v>22</v>
       </c>
-      <c r="D35" s="211"/>
-      <c r="E35" s="212"/>
-      <c r="F35" s="213"/>
+      <c r="D35" s="215"/>
+      <c r="E35" s="216"/>
+      <c r="F35" s="217"/>
     </row>
     <row r="36" spans="1:6" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -7212,9 +7215,9 @@
       <c r="C36">
         <v>16</v>
       </c>
-      <c r="D36" s="211"/>
-      <c r="E36" s="212"/>
-      <c r="F36" s="213"/>
+      <c r="D36" s="215"/>
+      <c r="E36" s="216"/>
+      <c r="F36" s="217"/>
     </row>
     <row r="37" spans="1:6" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -7226,9 +7229,9 @@
       <c r="C37">
         <v>21</v>
       </c>
-      <c r="D37" s="211"/>
-      <c r="E37" s="212"/>
-      <c r="F37" s="213"/>
+      <c r="D37" s="215"/>
+      <c r="E37" s="216"/>
+      <c r="F37" s="217"/>
     </row>
     <row r="38" spans="1:6" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -7240,9 +7243,9 @@
       <c r="C38">
         <v>17</v>
       </c>
-      <c r="D38" s="211"/>
-      <c r="E38" s="212"/>
-      <c r="F38" s="213"/>
+      <c r="D38" s="215"/>
+      <c r="E38" s="216"/>
+      <c r="F38" s="217"/>
     </row>
     <row r="39" spans="1:6" ht="12.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
@@ -7254,9 +7257,9 @@
       <c r="C39">
         <v>12</v>
       </c>
-      <c r="D39" s="214"/>
-      <c r="E39" s="215"/>
-      <c r="F39" s="216"/>
+      <c r="D39" s="218"/>
+      <c r="E39" s="219"/>
+      <c r="F39" s="220"/>
     </row>
     <row r="40" spans="1:6" ht="27.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -7268,11 +7271,11 @@
       <c r="C40" s="1">
         <v>0</v>
       </c>
-      <c r="D40" s="214" t="s">
+      <c r="D40" s="218" t="s">
         <v>1158</v>
       </c>
-      <c r="E40" s="215"/>
-      <c r="F40" s="216"/>
+      <c r="E40" s="219"/>
+      <c r="F40" s="220"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -7388,11 +7391,11 @@
       <c r="A1" s="106" t="s">
         <v>1125</v>
       </c>
-      <c r="B1" s="217" t="s">
+      <c r="B1" s="221" t="s">
         <v>970</v>
       </c>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
       <c r="E1" s="117" t="s">
         <v>0</v>
       </c>
@@ -7411,11 +7414,11 @@
       <c r="J1" s="107" t="s">
         <v>349</v>
       </c>
-      <c r="K1" s="218" t="s">
+      <c r="K1" s="222" t="s">
         <v>940</v>
       </c>
-      <c r="L1" s="218"/>
-      <c r="M1" s="218"/>
+      <c r="L1" s="222"/>
+      <c r="M1" s="222"/>
       <c r="N1" s="110"/>
       <c r="O1" s="121"/>
       <c r="S1" s="109"/>
@@ -8896,21 +8899,21 @@
       <c r="M51" s="142"/>
     </row>
     <row r="52" spans="1:19" ht="13" x14ac:dyDescent="0.25">
-      <c r="A52" s="219" t="s">
+      <c r="A52" s="223" t="s">
         <v>1093</v>
       </c>
-      <c r="B52" s="219"/>
-      <c r="C52" s="219"/>
-      <c r="D52" s="219"/>
-      <c r="E52" s="219"/>
-      <c r="F52" s="219"/>
-      <c r="G52" s="219"/>
-      <c r="H52" s="219"/>
-      <c r="I52" s="219"/>
-      <c r="J52" s="219"/>
-      <c r="K52" s="219"/>
-      <c r="L52" s="219"/>
-      <c r="M52" s="219"/>
+      <c r="B52" s="223"/>
+      <c r="C52" s="223"/>
+      <c r="D52" s="223"/>
+      <c r="E52" s="223"/>
+      <c r="F52" s="223"/>
+      <c r="G52" s="223"/>
+      <c r="H52" s="223"/>
+      <c r="I52" s="223"/>
+      <c r="J52" s="223"/>
+      <c r="K52" s="223"/>
+      <c r="L52" s="223"/>
+      <c r="M52" s="223"/>
     </row>
     <row r="53" spans="1:19" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="146" t="s">
@@ -10561,7 +10564,7 @@
     <mergeCell ref="A52:M52"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:K1 A2:M51 A52 A53:M91">
-    <cfRule type="containsBlanks" dxfId="22" priority="1">
+    <cfRule type="containsBlanks" dxfId="36" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15101,98 +15104,98 @@
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="96">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="96">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:H76">
-    <cfRule type="containsBlanks" dxfId="20" priority="2">
+    <cfRule type="containsBlanks" dxfId="34" priority="2">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77:I77">
-    <cfRule type="containsBlanks" dxfId="19" priority="88">
+    <cfRule type="containsBlanks" dxfId="33" priority="88">
       <formula>LEN(TRIM(A77))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="95">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="95">
       <formula>LEN(TRIM(C1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:H76">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="1">
       <formula>LEN(TRIM(F1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F77:I77">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="91">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="91">
       <formula>LEN(TRIM(F77))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35:I35 A78:H252 G117:I117 H144:I144 G151:I151 G155:I155">
-    <cfRule type="containsBlanks" dxfId="15" priority="98">
+    <cfRule type="containsBlanks" dxfId="29" priority="98">
       <formula>LEN(TRIM(A35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I34">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="66">
       <formula>LEN(TRIM(I2))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="13" priority="67">
+    <cfRule type="containsBlanks" dxfId="27" priority="67">
       <formula>LEN(TRIM(I2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:I76">
-    <cfRule type="containsBlanks" dxfId="12" priority="49">
+    <cfRule type="containsBlanks" dxfId="26" priority="49">
       <formula>LEN(TRIM(I36))=0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="11" priority="50">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="50">
       <formula>LEN(TRIM(I36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I78:I116">
-    <cfRule type="containsBlanks" dxfId="10" priority="37">
+    <cfRule type="containsBlanks" dxfId="24" priority="37">
       <formula>LEN(TRIM(I78))=0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="9" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="38">
       <formula>LEN(TRIM(I78))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I118:I143">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="25">
       <formula>LEN(TRIM(I118))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="7" priority="26">
+    <cfRule type="containsBlanks" dxfId="21" priority="26">
       <formula>LEN(TRIM(I118))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I145:I150">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="13">
       <formula>LEN(TRIM(I145))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="5" priority="14">
+    <cfRule type="containsBlanks" dxfId="19" priority="14">
       <formula>LEN(TRIM(I145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I152:I154">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="9">
       <formula>LEN(TRIM(I152))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="3" priority="10">
+    <cfRule type="containsBlanks" dxfId="17" priority="10">
       <formula>LEN(TRIM(I152))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I156:I252">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="3">
       <formula>LEN(TRIM(I156))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="1" priority="4">
+    <cfRule type="containsBlanks" dxfId="15" priority="4">
       <formula>LEN(TRIM(I156))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:K1 M1 H35:I35 F78:H1048576 G117:I117 H144:I144 G151:I151 G155:I155">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="97">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="97">
       <formula>LEN(TRIM(F1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16191,8 +16194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45ACF3F8-232A-4D9A-B3A7-867E85FEF5C0}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16239,7 +16242,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="105" t="s">
         <v>338</v>
       </c>
       <c r="B4" s="105" t="s">
@@ -16305,7 +16308,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="105" t="s">
         <v>350</v>
       </c>
       <c r="B10" s="105" t="s">
@@ -16316,7 +16319,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="105" t="s">
         <v>352</v>
       </c>
       <c r="B11" s="105" t="s">
@@ -16327,7 +16330,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="105" t="s">
         <v>354</v>
       </c>
       <c r="B12" s="105" t="s">
@@ -16360,7 +16363,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="105" t="s">
         <v>360</v>
       </c>
       <c r="B15" s="105" t="s">
@@ -16371,7 +16374,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="105" t="s">
         <v>362</v>
       </c>
       <c r="B16" s="105" t="s">
@@ -16404,7 +16407,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="105" t="s">
         <v>367</v>
       </c>
       <c r="B19" s="105" t="s">
@@ -16426,7 +16429,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="105" t="s">
         <v>370</v>
       </c>
       <c r="B21" s="105" t="s">
@@ -16469,19 +16472,19 @@
         <v>565</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="A25" s="105" t="s">
         <v>376</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="105" t="s">
         <v>430</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>566</v>
+      <c r="C25" s="103" t="s">
+        <v>1171</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="105" t="s">
         <v>377</v>
       </c>
       <c r="B26" s="105" t="s">
@@ -16492,7 +16495,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="105" t="s">
         <v>379</v>
       </c>
       <c r="B27" s="105" t="s">
@@ -16503,7 +16506,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="105" t="s">
         <v>381</v>
       </c>
       <c r="B28" s="105" t="s">
@@ -16514,7 +16517,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="105" t="s">
         <v>383</v>
       </c>
       <c r="B29" s="105" t="s">
@@ -16558,7 +16561,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="105" t="s">
         <v>389</v>
       </c>
       <c r="B33" s="105" t="s">
@@ -16569,7 +16572,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="105" t="s">
         <v>391</v>
       </c>
       <c r="B34" s="105" t="s">
@@ -16591,7 +16594,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="105" t="s">
         <v>395</v>
       </c>
       <c r="B36" s="105" t="s">
@@ -16613,7 +16616,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="105" t="s">
         <v>397</v>
       </c>
       <c r="B38" s="105" t="s">
@@ -16624,7 +16627,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="105" t="s">
         <v>399</v>
       </c>
       <c r="B39" s="105" t="s">
@@ -16646,7 +16649,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="105" t="s">
         <v>401</v>
       </c>
       <c r="B41" s="105" t="s">
@@ -16657,7 +16660,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="105" t="s">
         <v>403</v>
       </c>
       <c r="B42" s="105" t="s">
@@ -16679,7 +16682,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="105" t="s">
         <v>405</v>
       </c>
       <c r="B44" s="105" t="s">
@@ -16690,7 +16693,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="105" t="s">
         <v>407</v>
       </c>
       <c r="B45" s="105" t="s">
@@ -16723,7 +16726,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="105" t="s">
         <v>413</v>
       </c>
       <c r="B48" s="105" t="s">
@@ -16734,7 +16737,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="105" t="s">
         <v>415</v>
       </c>
       <c r="B49" s="105" t="s">
@@ -16767,7 +16770,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="105" t="s">
         <v>543</v>
       </c>
       <c r="B52" s="105" t="s">
@@ -16855,33 +16858,33 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="224" t="s">
+      <c r="A60" s="208" t="s">
         <v>1167</v>
       </c>
-      <c r="B60" s="225" t="s">
+      <c r="B60" s="209" t="s">
         <v>1168</v>
       </c>
-      <c r="C60" s="222" t="s">
+      <c r="C60" s="224" t="s">
         <v>1170</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="226" t="s">
+      <c r="A61" s="210" t="s">
         <v>1167</v>
       </c>
-      <c r="B61" s="227" t="s">
+      <c r="B61" s="211" t="s">
         <v>1056</v>
       </c>
-      <c r="C61" s="222"/>
+      <c r="C61" s="224"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="224" t="s">
+      <c r="A62" s="208" t="s">
         <v>1167</v>
       </c>
-      <c r="B62" s="225" t="s">
+      <c r="B62" s="209" t="s">
         <v>1169</v>
       </c>
-      <c r="C62" s="223"/>
+      <c r="C62" s="225"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -17206,11 +17209,11 @@
       <c r="D32" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="220" t="s">
+      <c r="A35" s="226" t="s">
         <v>1027</v>
       </c>
-      <c r="B35" s="221"/>
-      <c r="C35" s="221"/>
+      <c r="B35" s="227"/>
+      <c r="C35" s="227"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">

</xml_diff>